<commit_message>
feat(jupyter): Add tenant creation and module enabling support
- Add create_tenant() method to CRSLoader for creating tenants via MDMS v2 API
- Add _enable_module_for_tenant() to add tenants to citymodule config
- Add _update_citymodule_db() using psycopg2 for direct DB updates
- Update read_tenant_branding() to format for common-masters.StateInfo schema
- Add MinIO URL translation for external access (minio:9000 -> localhost:19000)
- Update DataLoader_v2.ipynb with new tenant creation cells

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/jupyter/dataloader/templates/Employee_Master_Dynamic_statea.xlsx
+++ b/jupyter/dataloader/templates/Employee_Master_Dynamic_statea.xlsx
@@ -62,7 +62,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
@@ -87,6 +87,18 @@
         <bgColor rgb="00FFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFC7CE"/>
+        <bgColor rgb="00FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C6EFCE"/>
+        <bgColor rgb="00C6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -100,7 +112,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -114,6 +126,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -904,17 +918,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>SANATION DEPARTMENT</t>
+          <t>WATER DEPARTMENT</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Engineer</t>
+          <t>engineer</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Employee,PGR Viewer</t>
+          <t>EMPLOYEE,PGR_VIEWER</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -953,19 +967,15 @@
       <c r="N2" s="3" t="n">
         <v>45463</v>
       </c>
-      <c r="O2" s="10" t="inlineStr">
-        <is>
-          <t>EXISTS</t>
+      <c r="O2" s="12" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
         </is>
       </c>
       <c r="P2" t="n">
-        <v>400</v>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>User already exists for the entered mobile number. Use a different mobile number to proceed.</t>
-        </is>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="Q2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="M3" s="3" t="n"/>

</xml_diff>